<commit_message>
minor changes to essay play
</commit_message>
<xml_diff>
--- a/docs/0b_forms/essay plan.xlsx
+++ b/docs/0b_forms/essay plan.xlsx
@@ -5,11 +5,11 @@
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathantang/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathantang/Documents/OneDrive - Goldsmiths College/Year-2/2-Software_Projects/repo/docs/0b_forms/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="6000" windowWidth="33600" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="90">
   <si>
     <t>Abstract</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Acknowledgements</t>
   </si>
   <si>
-    <t>Introduction</t>
-  </si>
-  <si>
     <r>
       <t>-</t>
     </r>
@@ -150,9 +147,6 @@
     </r>
   </si>
   <si>
-    <t>Background and Literature Review</t>
-  </si>
-  <si>
     <r>
       <t>-</t>
     </r>
@@ -249,9 +243,6 @@
     </r>
   </si>
   <si>
-    <t>Project Management Processes</t>
-  </si>
-  <si>
     <r>
       <t>-</t>
     </r>
@@ -324,9 +315,6 @@
     </r>
   </si>
   <si>
-    <t>Requirements</t>
-  </si>
-  <si>
     <r>
       <t>-</t>
     </r>
@@ -447,9 +435,6 @@
     </r>
   </si>
   <si>
-    <t>Design</t>
-  </si>
-  <si>
     <r>
       <t>-</t>
     </r>
@@ -618,9 +603,6 @@
     </r>
   </si>
   <si>
-    <t>Implementation</t>
-  </si>
-  <si>
     <r>
       <t>-</t>
     </r>
@@ -765,9 +747,6 @@
     </r>
   </si>
   <si>
-    <t>Testing &amp; Quality Assurance</t>
-  </si>
-  <si>
     <r>
       <t>-</t>
     </r>
@@ -1032,9 +1011,6 @@
     </r>
   </si>
   <si>
-    <t>Project evaluation</t>
-  </si>
-  <si>
     <r>
       <t>-</t>
     </r>
@@ -1206,35 +1182,35 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">       </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Development Methodology</t>
-    </r>
+    <t>1. Introduction</t>
+  </si>
+  <si>
+    <t>2. Background and Literature Review</t>
+  </si>
+  <si>
+    <t>3. Project Management Processes</t>
+  </si>
+  <si>
+    <t>4. Requirements</t>
+  </si>
+  <si>
+    <t>5. Design</t>
+  </si>
+  <si>
+    <t>6. Implementation</t>
+  </si>
+  <si>
+    <t>7. Testing &amp; Quality Assurance</t>
+  </si>
+  <si>
+    <t>8. Project evaluation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1291,8 +1267,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1305,6 +1288,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1315,7 +1303,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1327,8 +1315,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1378,8 +1367,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="11" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="12">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1390,6 +1382,7 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Neutral" xfId="11" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1670,8 +1663,8 @@
   </sheetPr>
   <dimension ref="A1:AT82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="161" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="115" zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1723,124 +1716,124 @@
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.2">
       <c r="E2" s="10" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="M2" s="10" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="N2" s="10" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="Q2" s="10" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="R2" s="10" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="S2" s="10" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="T2" s="10" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="U2" s="10" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="V2" s="10" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="W2" s="10" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="X2" s="10" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="Y2" s="10" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="Z2" s="10" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="AA2" s="10" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="AB2" s="10" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="AC2" s="10" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="AD2" s="10" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="AE2" s="10" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="AF2" s="10" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="AG2" s="10" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="AH2" s="10" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="AI2" s="10" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="AJ2" s="10" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="AK2" s="10" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="AL2" s="10" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="AM2" s="10" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="AN2" s="10" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="AO2" s="10" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="AP2" s="10" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:46" s="4" customFormat="1" ht="50" x14ac:dyDescent="0.2">
       <c r="C3" s="7"/>
       <c r="D3" s="7" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E3" s="8">
         <v>43547</v>
@@ -1965,7 +1958,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="X4" s="17">
         <v>2</v>
@@ -1975,7 +1968,7 @@
     <row r="5" spans="1:46" x14ac:dyDescent="0.2">
       <c r="B5" s="1"/>
       <c r="AR5" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="AT5" s="5"/>
     </row>
@@ -1992,10 +1985,10 @@
       <c r="Y6" s="17"/>
       <c r="AO6" s="11"/>
       <c r="AR6" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="AS6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="AT6" s="5"/>
     </row>
@@ -2012,10 +2005,10 @@
       <c r="Y7" s="17"/>
       <c r="AO7" s="11"/>
       <c r="AR7" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="AS7" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="AT7" s="5"/>
     </row>
@@ -2032,10 +2025,10 @@
       <c r="Y8" s="17"/>
       <c r="AO8" s="11"/>
       <c r="AR8" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="AS8" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="AT8" s="5"/>
     </row>
@@ -2052,20 +2045,20 @@
       <c r="Y9" s="17"/>
       <c r="AO9" s="11"/>
       <c r="AR9" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="AS9" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="AT9" s="5"/>
     </row>
     <row r="10" spans="1:46" x14ac:dyDescent="0.2">
       <c r="B10" s="1"/>
       <c r="AR10" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="AS10" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="AT10" s="5"/>
     </row>
@@ -2077,7 +2070,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="X11" s="17">
         <v>2</v>
@@ -2089,7 +2082,7 @@
     </row>
     <row r="13" spans="1:46" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>6</v>
+        <v>82</v>
       </c>
       <c r="S13" s="17">
         <v>2</v>
@@ -2106,10 +2099,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="S14" s="17">
         <v>2</v>
@@ -2126,10 +2119,10 @@
         <v>1</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="S15" s="17">
         <v>2</v>
@@ -2146,10 +2139,10 @@
         <v>1</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="S16" s="17">
         <v>2</v>
@@ -2166,10 +2159,10 @@
         <v>1</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="S17" s="17">
         <v>2</v>
@@ -2186,7 +2179,7 @@
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>11</v>
+        <v>83</v>
       </c>
       <c r="L19" s="17">
         <v>1</v>
@@ -2203,10 +2196,10 @@
         <v>1</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="L20" s="17">
         <v>1</v>
@@ -2223,10 +2216,10 @@
         <v>1</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="L21" s="17">
         <v>1</v>
@@ -2243,10 +2236,10 @@
         <v>1</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="L22" s="17">
         <v>1</v>
@@ -2263,10 +2256,10 @@
         <v>1</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="L23" s="17">
         <v>1</v>
@@ -2283,17 +2276,17 @@
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L25" s="17">
-        <v>1</v>
-      </c>
-      <c r="M25" s="17"/>
-      <c r="N25" s="17"/>
-      <c r="O25" s="17"/>
-      <c r="P25" s="17"/>
-      <c r="Q25" s="17"/>
-      <c r="R25" s="17"/>
+        <v>84</v>
+      </c>
+      <c r="L25" s="19">
+        <v>1</v>
+      </c>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="19"/>
+      <c r="P25" s="19"/>
+      <c r="Q25" s="19"/>
+      <c r="R25" s="19"/>
       <c r="S25" s="6"/>
       <c r="T25" s="6"/>
     </row>
@@ -2301,21 +2294,19 @@
       <c r="A26">
         <v>1</v>
       </c>
-      <c r="B26" s="16" t="s">
-        <v>90</v>
-      </c>
+      <c r="B26" s="16"/>
       <c r="C26" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="L26" s="17">
-        <v>1</v>
-      </c>
-      <c r="M26" s="17"/>
-      <c r="N26" s="17"/>
-      <c r="O26" s="17"/>
-      <c r="P26" s="17"/>
-      <c r="Q26" s="17"/>
-      <c r="R26" s="17"/>
+        <v>50</v>
+      </c>
+      <c r="L26" s="19">
+        <v>1</v>
+      </c>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="19"/>
+      <c r="Q26" s="19"/>
+      <c r="R26" s="19"/>
       <c r="S26" s="6"/>
       <c r="T26" s="6"/>
     </row>
@@ -2324,20 +2315,20 @@
         <v>1</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="L27" s="17">
-        <v>1</v>
-      </c>
-      <c r="M27" s="17"/>
-      <c r="N27" s="17"/>
-      <c r="O27" s="17"/>
-      <c r="P27" s="17"/>
-      <c r="Q27" s="17"/>
-      <c r="R27" s="17"/>
+        <v>50</v>
+      </c>
+      <c r="L27" s="19">
+        <v>1</v>
+      </c>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="19"/>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="19"/>
       <c r="S27" s="6"/>
       <c r="T27" s="6"/>
     </row>
@@ -2346,20 +2337,20 @@
         <v>1</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="L28" s="17">
-        <v>1</v>
-      </c>
-      <c r="M28" s="17"/>
-      <c r="N28" s="17"/>
-      <c r="O28" s="17"/>
-      <c r="P28" s="17"/>
-      <c r="Q28" s="17"/>
-      <c r="R28" s="17"/>
+        <v>50</v>
+      </c>
+      <c r="L28" s="19">
+        <v>1</v>
+      </c>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="19"/>
+      <c r="P28" s="19"/>
+      <c r="Q28" s="19"/>
+      <c r="R28" s="19"/>
       <c r="S28" s="6"/>
       <c r="T28" s="6"/>
     </row>
@@ -2368,20 +2359,20 @@
         <v>1</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="L29" s="17">
-        <v>1</v>
-      </c>
-      <c r="M29" s="17"/>
-      <c r="N29" s="17"/>
-      <c r="O29" s="17"/>
-      <c r="P29" s="17"/>
-      <c r="Q29" s="17"/>
-      <c r="R29" s="17"/>
+        <v>50</v>
+      </c>
+      <c r="L29" s="19">
+        <v>1</v>
+      </c>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="19"/>
+      <c r="P29" s="19"/>
+      <c r="Q29" s="19"/>
+      <c r="R29" s="19"/>
       <c r="S29" s="6"/>
       <c r="T29" s="6"/>
     </row>
@@ -2390,7 +2381,7 @@
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="L31" s="17">
         <v>1</v>
@@ -2407,10 +2398,10 @@
         <v>1</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="L32" s="17">
         <v>1</v>
@@ -2427,10 +2418,10 @@
         <v>1</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="L33" s="17">
         <v>1</v>
@@ -2447,67 +2438,67 @@
         <v>1</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="L34" s="17">
-        <v>1</v>
-      </c>
-      <c r="M34" s="17"/>
-      <c r="N34" s="17"/>
-      <c r="O34" s="17"/>
-      <c r="P34" s="17"/>
-      <c r="Q34" s="17"/>
-      <c r="R34" s="17"/>
+        <v>61</v>
+      </c>
+      <c r="L34" s="19">
+        <v>1</v>
+      </c>
+      <c r="M34" s="19"/>
+      <c r="N34" s="19"/>
+      <c r="O34" s="19"/>
+      <c r="P34" s="19"/>
+      <c r="Q34" s="19"/>
+      <c r="R34" s="19"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="L35" s="17">
-        <v>1</v>
-      </c>
-      <c r="M35" s="17"/>
-      <c r="N35" s="17"/>
-      <c r="O35" s="17"/>
-      <c r="P35" s="17"/>
-      <c r="Q35" s="17"/>
-      <c r="R35" s="17"/>
+        <v>61</v>
+      </c>
+      <c r="L35" s="19">
+        <v>1</v>
+      </c>
+      <c r="M35" s="19"/>
+      <c r="N35" s="19"/>
+      <c r="O35" s="19"/>
+      <c r="P35" s="19"/>
+      <c r="Q35" s="19"/>
+      <c r="R35" s="19"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="L36" s="17">
-        <v>1</v>
-      </c>
-      <c r="M36" s="17"/>
-      <c r="N36" s="17"/>
-      <c r="O36" s="17"/>
-      <c r="P36" s="17"/>
-      <c r="Q36" s="17"/>
-      <c r="R36" s="17"/>
+        <v>61</v>
+      </c>
+      <c r="L36" s="19">
+        <v>1</v>
+      </c>
+      <c r="M36" s="19"/>
+      <c r="N36" s="19"/>
+      <c r="O36" s="19"/>
+      <c r="P36" s="19"/>
+      <c r="Q36" s="19"/>
+      <c r="R36" s="19"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B37" s="1"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>26</v>
+        <v>86</v>
       </c>
       <c r="L38" s="17">
         <v>1</v>
@@ -2524,10 +2515,10 @@
         <v>1</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="L39" s="17">
         <v>1</v>
@@ -2541,7 +2532,7 @@
     </row>
     <row r="40" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="B40" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="L40" s="17">
         <v>1</v>
@@ -2555,7 +2546,7 @@
     </row>
     <row r="41" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="B41" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="L41" s="17">
         <v>1</v>
@@ -2569,7 +2560,7 @@
     </row>
     <row r="42" spans="1:18" ht="17" x14ac:dyDescent="0.2">
       <c r="B42" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="L42" s="17">
         <v>1</v>
@@ -2586,30 +2577,30 @@
         <v>1</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="L43" s="17">
-        <v>1</v>
-      </c>
-      <c r="M43" s="17"/>
-      <c r="N43" s="17"/>
-      <c r="O43" s="17"/>
-      <c r="P43" s="17"/>
-      <c r="Q43" s="17"/>
-      <c r="R43" s="17"/>
+        <v>58</v>
+      </c>
+      <c r="L43" s="19">
+        <v>1</v>
+      </c>
+      <c r="M43" s="19"/>
+      <c r="N43" s="19"/>
+      <c r="O43" s="19"/>
+      <c r="P43" s="19"/>
+      <c r="Q43" s="19"/>
+      <c r="R43" s="19"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="L44" s="17">
         <v>1</v>
@@ -2626,47 +2617,47 @@
         <v>1</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="L45" s="17">
-        <v>1</v>
-      </c>
-      <c r="M45" s="17"/>
-      <c r="N45" s="17"/>
-      <c r="O45" s="17"/>
-      <c r="P45" s="17"/>
-      <c r="Q45" s="17"/>
-      <c r="R45" s="17"/>
+        <v>61</v>
+      </c>
+      <c r="L45" s="19">
+        <v>1</v>
+      </c>
+      <c r="M45" s="19"/>
+      <c r="N45" s="19"/>
+      <c r="O45" s="19"/>
+      <c r="P45" s="19"/>
+      <c r="Q45" s="19"/>
+      <c r="R45" s="19"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="L46" s="17">
-        <v>1</v>
-      </c>
-      <c r="M46" s="17"/>
-      <c r="N46" s="17"/>
-      <c r="O46" s="17"/>
-      <c r="P46" s="17"/>
-      <c r="Q46" s="17"/>
-      <c r="R46" s="17"/>
+        <v>58</v>
+      </c>
+      <c r="L46" s="19">
+        <v>1</v>
+      </c>
+      <c r="M46" s="19"/>
+      <c r="N46" s="19"/>
+      <c r="O46" s="19"/>
+      <c r="P46" s="19"/>
+      <c r="Q46" s="19"/>
+      <c r="R46" s="19"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B47" s="1"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.2">
@@ -2674,10 +2665,10 @@
         <v>1</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="S49" s="17">
         <v>2</v>
@@ -2694,10 +2685,10 @@
         <v>1</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="S50" s="17">
         <v>2</v>
@@ -2714,10 +2705,10 @@
         <v>1</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="S51" s="17">
         <v>2</v>
@@ -2734,10 +2725,10 @@
         <v>1</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="S52" s="17">
         <v>2</v>
@@ -2754,10 +2745,10 @@
         <v>1</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="S53" s="17">
         <v>2</v>
@@ -2774,10 +2765,10 @@
         <v>1</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="S54" s="17">
         <v>2</v>
@@ -2794,7 +2785,7 @@
     </row>
     <row r="56" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B56" s="1" t="s">
-        <v>41</v>
+        <v>88</v>
       </c>
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.2">
@@ -2802,10 +2793,10 @@
         <v>1</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="S57" s="17">
         <v>2</v>
@@ -2819,7 +2810,7 @@
     </row>
     <row r="58" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="B58" s="3" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="S58" s="17">
         <v>2</v>
@@ -2833,7 +2824,7 @@
     </row>
     <row r="59" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="B59" s="3" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="S59" s="17">
         <v>2</v>
@@ -2847,7 +2838,7 @@
     </row>
     <row r="60" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="B60" s="3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="S60" s="17">
         <v>2</v>
@@ -2861,7 +2852,7 @@
     </row>
     <row r="61" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="B61" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="S61" s="17">
         <v>2</v>
@@ -2875,7 +2866,7 @@
     </row>
     <row r="62" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="B62" s="3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="S62" s="17">
         <v>2</v>
@@ -2889,7 +2880,7 @@
     </row>
     <row r="63" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="B63" s="3" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="S63" s="17">
         <v>2</v>
@@ -2906,10 +2897,10 @@
         <v>1</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="S64" s="17">
         <v>2</v>
@@ -2926,10 +2917,10 @@
         <v>1</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="S65" s="17">
         <v>2</v>
@@ -2946,10 +2937,10 @@
         <v>1</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C66" s="12" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="S66" s="17">
         <v>2</v>
@@ -2966,10 +2957,10 @@
         <v>1</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="S67" s="17">
         <v>2</v>
@@ -2986,7 +2977,7 @@
     </row>
     <row r="69" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B69" s="1" t="s">
-        <v>53</v>
+        <v>89</v>
       </c>
       <c r="S69" s="17">
         <v>2</v>
@@ -3003,7 +2994,7 @@
         <v>1</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="S70" s="17">
         <v>2</v>
@@ -3020,10 +3011,10 @@
         <v>1</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C71" s="12" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="S71" s="17">
         <v>2</v>
@@ -3040,15 +3031,15 @@
     </row>
     <row r="73" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B73" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="74" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B74" s="1" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C74" s="12" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="L74" s="17">
         <v>1</v>
@@ -3062,10 +3053,10 @@
     </row>
     <row r="75" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B75" s="1" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C75" s="12" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="L75" s="17">
         <v>1</v>
@@ -3079,10 +3070,10 @@
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B76" s="1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C76" s="13" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="L76" s="17">
         <v>1</v>
@@ -3096,10 +3087,10 @@
     </row>
     <row r="77" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B77" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C77" s="13" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="L77" s="17">
         <v>1</v>
@@ -3113,10 +3104,10 @@
     </row>
     <row r="78" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B78" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C78" s="13" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="L78" s="17">
         <v>1</v>
@@ -3130,10 +3121,10 @@
     </row>
     <row r="79" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B79" s="1" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C79" s="13" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="L79" s="17">
         <v>1</v>
@@ -3147,10 +3138,10 @@
     </row>
     <row r="80" spans="1:25" x14ac:dyDescent="0.2">
       <c r="B80" s="1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C80" s="15" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="S80" s="17">
         <v>2</v>
@@ -3167,46 +3158,27 @@
         <v>0</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="L75:R75"/>
-    <mergeCell ref="L76:R76"/>
-    <mergeCell ref="L77:R77"/>
-    <mergeCell ref="L78:R78"/>
-    <mergeCell ref="L79:R79"/>
-    <mergeCell ref="S59:Y59"/>
-    <mergeCell ref="S60:Y60"/>
-    <mergeCell ref="S61:Y61"/>
-    <mergeCell ref="S62:Y62"/>
-    <mergeCell ref="L74:R74"/>
-    <mergeCell ref="S70:Y70"/>
-    <mergeCell ref="S71:Y71"/>
-    <mergeCell ref="S63:Y63"/>
-    <mergeCell ref="S64:Y64"/>
-    <mergeCell ref="S65:Y65"/>
-    <mergeCell ref="S66:Y66"/>
-    <mergeCell ref="S67:Y67"/>
-    <mergeCell ref="S69:Y69"/>
-    <mergeCell ref="S50:Y50"/>
-    <mergeCell ref="S51:Y51"/>
-    <mergeCell ref="S52:Y52"/>
-    <mergeCell ref="S53:Y53"/>
-    <mergeCell ref="S58:Y58"/>
-    <mergeCell ref="S57:Y57"/>
-    <mergeCell ref="S54:Y54"/>
-    <mergeCell ref="L39:R39"/>
-    <mergeCell ref="L40:R40"/>
-    <mergeCell ref="L41:R41"/>
-    <mergeCell ref="L28:R28"/>
-    <mergeCell ref="L44:R44"/>
-    <mergeCell ref="S16:Y16"/>
-    <mergeCell ref="S17:Y17"/>
-    <mergeCell ref="L36:R36"/>
-    <mergeCell ref="L33:R33"/>
-    <mergeCell ref="L38:R38"/>
+    <mergeCell ref="S80:Y80"/>
+    <mergeCell ref="L27:R27"/>
+    <mergeCell ref="L1:R1"/>
+    <mergeCell ref="S1:Y1"/>
+    <mergeCell ref="Z1:AF1"/>
+    <mergeCell ref="L23:R23"/>
+    <mergeCell ref="L25:R25"/>
+    <mergeCell ref="L26:R26"/>
+    <mergeCell ref="L29:R29"/>
+    <mergeCell ref="L31:R31"/>
+    <mergeCell ref="L32:R32"/>
+    <mergeCell ref="L34:R34"/>
+    <mergeCell ref="L35:R35"/>
+    <mergeCell ref="L42:R42"/>
+    <mergeCell ref="L43:R43"/>
+    <mergeCell ref="L45:R45"/>
     <mergeCell ref="S49:Y49"/>
     <mergeCell ref="AG1:AO1"/>
     <mergeCell ref="L19:R19"/>
@@ -3223,22 +3195,41 @@
     <mergeCell ref="S13:Y13"/>
     <mergeCell ref="S14:Y14"/>
     <mergeCell ref="S15:Y15"/>
-    <mergeCell ref="S80:Y80"/>
-    <mergeCell ref="L27:R27"/>
-    <mergeCell ref="L1:R1"/>
-    <mergeCell ref="S1:Y1"/>
-    <mergeCell ref="Z1:AF1"/>
-    <mergeCell ref="L23:R23"/>
-    <mergeCell ref="L25:R25"/>
-    <mergeCell ref="L26:R26"/>
-    <mergeCell ref="L29:R29"/>
-    <mergeCell ref="L31:R31"/>
-    <mergeCell ref="L32:R32"/>
-    <mergeCell ref="L34:R34"/>
-    <mergeCell ref="L35:R35"/>
-    <mergeCell ref="L42:R42"/>
-    <mergeCell ref="L43:R43"/>
-    <mergeCell ref="L45:R45"/>
+    <mergeCell ref="S16:Y16"/>
+    <mergeCell ref="S17:Y17"/>
+    <mergeCell ref="L36:R36"/>
+    <mergeCell ref="L33:R33"/>
+    <mergeCell ref="L38:R38"/>
+    <mergeCell ref="L39:R39"/>
+    <mergeCell ref="L40:R40"/>
+    <mergeCell ref="L41:R41"/>
+    <mergeCell ref="L28:R28"/>
+    <mergeCell ref="L44:R44"/>
+    <mergeCell ref="S50:Y50"/>
+    <mergeCell ref="S51:Y51"/>
+    <mergeCell ref="S52:Y52"/>
+    <mergeCell ref="S53:Y53"/>
+    <mergeCell ref="S58:Y58"/>
+    <mergeCell ref="S57:Y57"/>
+    <mergeCell ref="S54:Y54"/>
+    <mergeCell ref="S59:Y59"/>
+    <mergeCell ref="S60:Y60"/>
+    <mergeCell ref="S61:Y61"/>
+    <mergeCell ref="S62:Y62"/>
+    <mergeCell ref="L74:R74"/>
+    <mergeCell ref="S70:Y70"/>
+    <mergeCell ref="S71:Y71"/>
+    <mergeCell ref="S63:Y63"/>
+    <mergeCell ref="S64:Y64"/>
+    <mergeCell ref="S65:Y65"/>
+    <mergeCell ref="S66:Y66"/>
+    <mergeCell ref="S67:Y67"/>
+    <mergeCell ref="S69:Y69"/>
+    <mergeCell ref="L75:R75"/>
+    <mergeCell ref="L76:R76"/>
+    <mergeCell ref="L77:R77"/>
+    <mergeCell ref="L78:R78"/>
+    <mergeCell ref="L79:R79"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>

</xml_diff>